<commit_message>
new data taken at mid mount
</commit_message>
<xml_diff>
--- a/robots/jackal/vision_based_navigation_ttt/tau_values/tau_value1.xlsx
+++ b/robots/jackal/vision_based_navigation_ttt/tau_values/tau_value1.xlsx
@@ -348,19 +348,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1">
-        <v>1.169185096264388</v>
+        <v>3.026113033294678</v>
       </c>
       <c r="B1">
-        <v>2.358443848387898</v>
+        <v>6.359650611877441</v>
       </c>
       <c r="C1">
-        <v>2.702661365852998</v>
+        <v>7.085855960845947</v>
       </c>
       <c r="D1">
-        <v>1.929790039302267</v>
+        <v>7.611157894134521</v>
       </c>
       <c r="E1">
-        <v>0.8039147470588185</v>
+        <v>4.642078399658203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>